<commit_message>
Agrego correcciones clase 3
</commit_message>
<xml_diff>
--- a/Ejercicios_Clase_3_Link_Plofi.xlsx
+++ b/Ejercicios_Clase_3_Link_Plofi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bussolaf\Desktop\FLOR - NO BORRAR\Curso PROGRMACION\Ejercicios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0A75762B-F77B-4AEC-BC9E-4903C7CB083E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E24B4CE1-2BEA-47A2-9568-8A36AA70C2F6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="10" activeTab="13" xr2:uid="{FEF5156E-0849-4B8D-853B-10D8FD0E8E0B}"/>
   </bookViews>
@@ -191,7 +191,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="243">
   <si>
     <t>Hacer un pseudocódigo que imprima los números del 1 al 100.</t>
   </si>
@@ -865,12 +865,245 @@
   <si>
     <t>#Esto se puede escribir como for n in range(1,5,+1)  ??? (pero después los n de los otros for cambiar a n2)</t>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF002060"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Respuesta en clase:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF002060"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Estoy generando el arreglo dentro del while y por lo tanto se está pisando cada vez que se reinicia.</t>
+    </r>
+  </si>
+  <si>
+    <t>arreglo_frases = []</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    arreglo_frases.append(input())</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF002060"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Corrección:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF002060"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Definir 1ro el array x fuera de manera global y después sumar elementos con .append()</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">#Este For debe estar por fuera para que </t>
+  </si>
+  <si>
+    <t>cuente una sóla vez y no por cada  introducción</t>
+  </si>
+  <si>
+    <t>o dentro del while sin el for:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cantidad_frases = cantidad_frases+1</t>
+  </si>
+  <si>
+    <t># Corrección en clase:</t>
+  </si>
+  <si>
+    <t>arreglo = []</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    arreglo.append(numeros_ingresados)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   if n &gt; numero_mayor:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        numero_mayor = n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   if n &lt; numero_menor:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       numero_menor = n</t>
+  </si>
+  <si>
+    <t>#Estos For ahora pueden estar por fuera para que 1ro se ingresen todos los números y después los compare, eso por cambiar el "while x un for"</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF002060"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>for</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> n in arreglo:</t>
+    </r>
+  </si>
+  <si>
+    <t>for numero in range(1,6)    #Este "numero" no va a ser el mismo porque es una "variable local"</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">numero_mayor = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF002060"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>None</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">numero_menor = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF002060"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>None</t>
+    </r>
+  </si>
+  <si>
+    <t>#Acá podemos decirle que sea ninguno o nada para arrancar sin un dato concreto que no tengo</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    if numero_mayor </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF002060"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">is None or </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>numero_ingresado &gt; numero_mayor:</t>
+    </r>
+  </si>
+  <si>
+    <t># Hago una comparación pero tengo que incluir al None para ver como se comporta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        numero_mayor = numero_ingresado</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    if numero_menor </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF002060"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">is None or </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>numero_ingresado &gt; numero_menor:</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">        numero_menor = numero_ingresado</t>
+  </si>
+  <si>
+    <t># Otra opción vista en clase sin array:</t>
+  </si>
+  <si>
+    <t>No se si  la correccion la hizo Plofi</t>
+  </si>
+  <si>
+    <t>instruccion en Pytho sería numero +=</t>
+  </si>
+  <si>
+    <t>aunque numero = numero + 1 tambien esta bien</t>
+  </si>
+  <si>
+    <t>solo que con += anda mas rápido y abreviado</t>
+  </si>
+  <si>
+    <t>Oscar Vasta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Solo agregaría que para sumar 1 al número la </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    numero_ingresado = int(input("Ingrese un número, imprimiremos el mayor y el menor de su serie de 5 números"))</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -913,9 +1146,31 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF002060"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF002060"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <strike/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF002060"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -953,7 +1208,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -975,8 +1230,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1372,8 +1636,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B7F379E-7728-4017-A165-84A99986BB7F}">
   <dimension ref="A1:K50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1523,7 +1787,7 @@
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
       <c r="J12" s="5"/>
-      <c r="K12" s="7" t="s">
+      <c r="K12" s="22" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1545,10 +1809,10 @@
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
-      <c r="J13" s="5" t="s">
+      <c r="J13" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="K13" s="6" t="s">
+      <c r="K13" s="20" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1570,10 +1834,10 @@
       <c r="G14" s="6"/>
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
-      <c r="J14" s="5" t="s">
+      <c r="J14" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="K14" s="6" t="s">
+      <c r="K14" s="20" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1603,9 +1867,11 @@
       <c r="F16" s="5"/>
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
-      <c r="K16" s="6"/>
+      <c r="I16" s="23"/>
+      <c r="J16" s="23" t="s">
+        <v>236</v>
+      </c>
+      <c r="K16" s="23"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
@@ -1618,9 +1884,11 @@
       <c r="F17" s="8"/>
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="6"/>
-      <c r="K17" s="6"/>
+      <c r="I17" s="23"/>
+      <c r="J17" s="23" t="s">
+        <v>241</v>
+      </c>
+      <c r="K17" s="23"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
@@ -1631,9 +1899,11 @@
       <c r="F18" s="7"/>
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="6"/>
-      <c r="K18" s="6"/>
+      <c r="I18" s="23"/>
+      <c r="J18" s="23" t="s">
+        <v>237</v>
+      </c>
+      <c r="K18" s="23"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
@@ -1644,9 +1914,11 @@
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="6"/>
+      <c r="I19" s="23"/>
+      <c r="J19" s="23" t="s">
+        <v>238</v>
+      </c>
+      <c r="K19" s="23"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
@@ -1657,9 +1929,11 @@
       <c r="F20" s="8"/>
       <c r="G20" s="6"/>
       <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="6"/>
-      <c r="K20" s="6"/>
+      <c r="I20" s="23"/>
+      <c r="J20" s="23" t="s">
+        <v>239</v>
+      </c>
+      <c r="K20" s="23"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
@@ -1670,9 +1944,11 @@
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
       <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="6"/>
-      <c r="K21" s="6"/>
+      <c r="I21" s="23"/>
+      <c r="J21" s="23" t="s">
+        <v>240</v>
+      </c>
+      <c r="K21" s="23"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="6"/>
@@ -1683,9 +1959,9 @@
       <c r="F22" s="8"/>
       <c r="G22" s="6"/>
       <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
-      <c r="J22" s="6"/>
-      <c r="K22" s="6"/>
+      <c r="I22" s="23"/>
+      <c r="J22" s="23"/>
+      <c r="K22" s="23"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
@@ -2276,7 +2552,7 @@
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
-      <c r="F17" s="18"/>
+      <c r="F17" s="17"/>
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
@@ -2296,7 +2572,7 @@
       <c r="B19" s="3"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
-      <c r="F19" s="18"/>
+      <c r="F19" s="17"/>
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
       <c r="I19" s="6"/>
@@ -3006,7 +3282,7 @@
       <c r="A20" s="6"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
-      <c r="F20" s="18"/>
+      <c r="F20" s="17"/>
       <c r="G20" s="6"/>
       <c r="H20" s="6"/>
       <c r="I20" s="6"/>
@@ -3026,7 +3302,7 @@
       <c r="B22" s="3"/>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
-      <c r="F22" s="18"/>
+      <c r="F22" s="17"/>
       <c r="G22" s="6"/>
       <c r="H22" s="6"/>
       <c r="I22" s="6"/>
@@ -3708,7 +3984,7 @@
       <c r="A20" s="6"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
-      <c r="F20" s="18"/>
+      <c r="F20" s="17"/>
       <c r="G20" s="6"/>
       <c r="H20" s="6"/>
       <c r="I20" s="6"/>
@@ -3728,7 +4004,7 @@
       <c r="B22" s="3"/>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
-      <c r="F22" s="18"/>
+      <c r="F22" s="17"/>
       <c r="G22" s="6"/>
       <c r="H22" s="6"/>
       <c r="I22" s="6"/>
@@ -4377,7 +4653,7 @@
       <c r="A20" s="6"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
-      <c r="F20" s="18"/>
+      <c r="F20" s="17"/>
       <c r="G20" s="6"/>
       <c r="H20" s="6"/>
       <c r="I20" s="6"/>
@@ -4397,7 +4673,7 @@
       <c r="B22" s="3"/>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
-      <c r="F22" s="18"/>
+      <c r="F22" s="17"/>
       <c r="G22" s="6"/>
       <c r="H22" s="6"/>
       <c r="I22" s="6"/>
@@ -4805,10 +5081,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{224859DA-39D0-4E0F-89C4-8EA1C04DE0FA}">
-  <dimension ref="A2:O58"/>
+  <dimension ref="A2:Q63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="N57" sqref="N57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4818,7 +5094,7 @@
     <col min="4" max="4" width="69.7109375" style="5" customWidth="1"/>
     <col min="5" max="5" width="3" style="5" bestFit="1" customWidth="1"/>
     <col min="6" max="9" width="11.42578125" style="5"/>
-    <col min="10" max="10" width="2.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="3.5703125" style="5" customWidth="1"/>
     <col min="11" max="16384" width="11.42578125" style="5"/>
   </cols>
   <sheetData>
@@ -5027,7 +5303,9 @@
       </c>
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
-      <c r="J15" s="1"/>
+      <c r="J15" s="19" t="s">
+        <v>217</v>
+      </c>
       <c r="K15" s="1"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
@@ -5047,7 +5325,7 @@
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
         <v>155</v>
       </c>
@@ -5063,8 +5341,15 @@
       </c>
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J17" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="L17" s="3"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
         <v>171</v>
       </c>
@@ -5079,8 +5364,15 @@
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>
       <c r="I18" s="6"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J18" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="K18" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="L18" s="3"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
         <v>172</v>
       </c>
@@ -5095,8 +5387,15 @@
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
       <c r="I19" s="6"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J19" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="K19" s="19" t="s">
+        <v>218</v>
+      </c>
+      <c r="L19" s="3"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
         <v>173</v>
       </c>
@@ -5113,8 +5412,11 @@
       <c r="G20" s="6"/>
       <c r="H20" s="6"/>
       <c r="I20" s="6"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J20" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
         <v>174</v>
       </c>
@@ -5131,8 +5433,15 @@
       <c r="G21" s="6"/>
       <c r="H21" s="6"/>
       <c r="I21" s="6"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J21" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="K21" s="19" t="s">
+        <v>226</v>
+      </c>
+      <c r="L21" s="3"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
         <v>175</v>
       </c>
@@ -5145,8 +5454,15 @@
       <c r="G22" s="6"/>
       <c r="H22" s="6"/>
       <c r="I22" s="6"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J22" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="K22" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="L22" s="3"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
         <v>176</v>
       </c>
@@ -5160,8 +5476,15 @@
       <c r="G23" s="6"/>
       <c r="H23" s="6"/>
       <c r="I23" s="6"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J23" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="K23" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="L23" s="3"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="14" t="s">
         <v>187</v>
       </c>
@@ -5179,8 +5502,14 @@
       <c r="G24" s="6"/>
       <c r="H24" s="6"/>
       <c r="I24" s="6"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J24" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="K24" s="19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
         <v>188</v>
       </c>
@@ -5196,8 +5525,11 @@
       <c r="G25" s="6"/>
       <c r="H25" s="6"/>
       <c r="I25" s="6"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J25" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="14" t="s">
         <v>189</v>
       </c>
@@ -5214,8 +5546,17 @@
       <c r="G26" s="6"/>
       <c r="H26" s="6"/>
       <c r="I26" s="6"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J26" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="K26" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="N26" s="19" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="6"/>
       <c r="C27" s="6"/>
       <c r="D27" s="6"/>
@@ -5228,8 +5569,18 @@
       <c r="G27" s="6"/>
       <c r="H27" s="6"/>
       <c r="I27" s="6"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J27" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="K27" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="L27" s="6"/>
+      <c r="M27" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="6"/>
       <c r="B28" s="10"/>
       <c r="C28" s="6"/>
@@ -5243,8 +5594,15 @@
       <c r="G28" s="6"/>
       <c r="H28" s="6"/>
       <c r="I28" s="6"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J28" s="14" t="s">
+        <v>171</v>
+      </c>
+      <c r="K28" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="L28" s="6"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
@@ -5258,8 +5616,13 @@
       <c r="G29" s="6"/>
       <c r="H29" s="6"/>
       <c r="I29" s="6"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J29" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="K29" s="10"/>
+      <c r="L29" s="6"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="6"/>
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
@@ -5269,8 +5632,15 @@
       <c r="G30" s="7"/>
       <c r="H30" s="6"/>
       <c r="I30" s="6"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J30" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="K30" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="L30" s="6"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="6"/>
       <c r="B31" s="6"/>
       <c r="C31" s="6"/>
@@ -5280,8 +5650,15 @@
       <c r="G31" s="6"/>
       <c r="H31" s="6"/>
       <c r="I31" s="6"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J31" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="K31" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="L31" s="6"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="6"/>
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
@@ -5291,8 +5668,15 @@
       <c r="G32" s="6"/>
       <c r="H32" s="6"/>
       <c r="I32" s="6"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J32" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="K32" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="L32" s="6"/>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="6"/>
       <c r="B33" s="6"/>
       <c r="C33" s="6"/>
@@ -5302,8 +5686,13 @@
       <c r="G33" s="6"/>
       <c r="H33" s="6"/>
       <c r="I33" s="6"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J33" s="14" t="s">
+        <v>176</v>
+      </c>
+      <c r="K33" s="6"/>
+      <c r="L33" s="6"/>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="6"/>
       <c r="B34" s="6"/>
       <c r="C34" s="6"/>
@@ -5313,8 +5702,15 @@
       <c r="G34" s="6"/>
       <c r="H34" s="6"/>
       <c r="I34" s="6"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J34" s="14" t="s">
+        <v>187</v>
+      </c>
+      <c r="K34" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="L34" s="6"/>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="6"/>
       <c r="B35" s="6"/>
       <c r="C35" s="6"/>
@@ -5324,8 +5720,15 @@
       <c r="G35" s="6"/>
       <c r="H35" s="6"/>
       <c r="I35" s="6"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J35" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="K35" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="L35" s="6"/>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" s="6"/>
       <c r="B36" s="10"/>
       <c r="C36" s="6"/>
@@ -5335,8 +5738,15 @@
       <c r="G36" s="7"/>
       <c r="H36" s="4"/>
       <c r="I36" s="6"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J36" s="14" t="s">
+        <v>189</v>
+      </c>
+      <c r="K36" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="L36" s="6"/>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" s="6"/>
       <c r="B37" s="6"/>
       <c r="C37" s="6"/>
@@ -5346,8 +5756,14 @@
       <c r="G37" s="6"/>
       <c r="H37" s="6"/>
       <c r="I37" s="6"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J37" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="K37" s="5" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
@@ -5357,8 +5773,10 @@
       <c r="G38" s="6"/>
       <c r="H38" s="6"/>
       <c r="I38" s="6"/>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J38" s="8"/>
+      <c r="L38" s="6"/>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
@@ -5369,9 +5787,9 @@
       <c r="H39" s="6"/>
       <c r="I39" s="6"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" s="6"/>
-      <c r="B40" s="6"/>
+      <c r="B40" s="10"/>
       <c r="C40" s="6"/>
       <c r="D40" s="6"/>
       <c r="E40" s="8"/>
@@ -5379,52 +5797,77 @@
       <c r="G40" s="6"/>
       <c r="H40" s="6"/>
       <c r="I40" s="6"/>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J40" s="19" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" s="6"/>
       <c r="B41" s="6"/>
       <c r="C41" s="6"/>
       <c r="D41" s="6"/>
-      <c r="E41" s="6"/>
+      <c r="E41" s="7"/>
       <c r="F41" s="6"/>
       <c r="G41" s="6"/>
       <c r="H41" s="6"/>
       <c r="I41" s="6"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" s="6"/>
-      <c r="B42" s="10"/>
+      <c r="B42" s="6"/>
       <c r="C42" s="6"/>
       <c r="D42" s="6"/>
-      <c r="E42" s="8"/>
+      <c r="E42" s="6"/>
       <c r="F42" s="6"/>
       <c r="G42" s="6"/>
       <c r="H42" s="6"/>
       <c r="I42" s="6"/>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J42" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="K42" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="L42" s="3"/>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" s="6"/>
       <c r="B43" s="6"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
-      <c r="E43" s="7"/>
+      <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
       <c r="H43" s="6"/>
       <c r="I43" s="6"/>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J43" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="K43" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="L43" s="3"/>
+      <c r="M43" s="19" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" s="6"/>
       <c r="B44" s="6"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
-      <c r="E44" s="6"/>
+      <c r="E44" s="8"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
       <c r="H44" s="6"/>
       <c r="I44" s="6"/>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J44" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="K44" s="19"/>
+      <c r="L44" s="3"/>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" s="6"/>
       <c r="B45" s="6"/>
       <c r="C45" s="6"/>
@@ -5434,63 +5877,104 @@
       <c r="G45" s="6"/>
       <c r="H45" s="6"/>
       <c r="I45" s="6"/>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J45" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K45" s="19" t="s">
+        <v>226</v>
+      </c>
+      <c r="L45" s="3"/>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46" s="6"/>
       <c r="B46" s="6"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="8"/>
       <c r="F46" s="6"/>
-      <c r="G46" s="6"/>
+      <c r="G46" s="7"/>
       <c r="H46" s="6"/>
       <c r="I46" s="6"/>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J46" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="K46" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="L46" s="3"/>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47" s="6"/>
       <c r="B47" s="6"/>
       <c r="C47" s="6"/>
       <c r="D47" s="6"/>
-      <c r="E47" s="6"/>
+      <c r="E47" s="7"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
       <c r="H47" s="6"/>
       <c r="I47" s="6"/>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J47" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="K47" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="Q47" s="19" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48" s="6"/>
       <c r="B48" s="6"/>
       <c r="C48" s="6"/>
       <c r="D48" s="6"/>
-      <c r="E48" s="8"/>
+      <c r="E48" s="6"/>
       <c r="F48" s="6"/>
-      <c r="G48" s="7"/>
+      <c r="G48" s="6"/>
       <c r="H48" s="6"/>
       <c r="I48" s="6"/>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J48" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="K48" s="5" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="6"/>
       <c r="B49" s="6"/>
       <c r="C49" s="6"/>
       <c r="D49" s="6"/>
-      <c r="E49" s="7"/>
+      <c r="E49" s="6"/>
       <c r="F49" s="6"/>
       <c r="G49" s="6"/>
       <c r="H49" s="6"/>
       <c r="I49" s="6"/>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J49" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="K49" s="5" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="6"/>
       <c r="B50" s="6"/>
       <c r="C50" s="6"/>
       <c r="D50" s="6"/>
-      <c r="E50" s="6"/>
+      <c r="E50" s="8"/>
       <c r="F50" s="6"/>
       <c r="G50" s="6"/>
       <c r="H50" s="6"/>
       <c r="I50" s="6"/>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J50" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="K50" s="5" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="6"/>
       <c r="B51" s="6"/>
       <c r="C51" s="6"/>
@@ -5500,19 +5984,28 @@
       <c r="G51" s="6"/>
       <c r="H51" s="6"/>
       <c r="I51" s="6"/>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J51" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="6"/>
       <c r="B52" s="6"/>
       <c r="C52" s="6"/>
       <c r="D52" s="6"/>
-      <c r="E52" s="8"/>
+      <c r="E52" s="6"/>
       <c r="F52" s="6"/>
-      <c r="G52" s="6"/>
+      <c r="G52" s="7"/>
       <c r="H52" s="6"/>
       <c r="I52" s="6"/>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J52" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="K52" s="5" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="6"/>
       <c r="B53" s="6"/>
       <c r="C53" s="6"/>
@@ -5522,19 +6015,31 @@
       <c r="G53" s="6"/>
       <c r="H53" s="6"/>
       <c r="I53" s="6"/>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J53" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="K53" s="5" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="6"/>
       <c r="B54" s="6"/>
       <c r="C54" s="6"/>
       <c r="D54" s="6"/>
       <c r="E54" s="6"/>
       <c r="F54" s="6"/>
-      <c r="G54" s="7"/>
+      <c r="G54" s="6"/>
       <c r="H54" s="6"/>
       <c r="I54" s="6"/>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J54" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="K54" s="5" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="6"/>
       <c r="B55" s="6"/>
       <c r="C55" s="6"/>
@@ -5544,8 +6049,14 @@
       <c r="G55" s="6"/>
       <c r="H55" s="6"/>
       <c r="I55" s="6"/>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J55" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="K55" s="5" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="6"/>
       <c r="B56" s="6"/>
       <c r="C56" s="6"/>
@@ -5555,28 +6066,28 @@
       <c r="G56" s="6"/>
       <c r="H56" s="6"/>
       <c r="I56" s="6"/>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57" s="6"/>
-      <c r="B57" s="6"/>
-      <c r="C57" s="6"/>
-      <c r="D57" s="6"/>
-      <c r="E57" s="6"/>
-      <c r="F57" s="6"/>
-      <c r="G57" s="6"/>
-      <c r="H57" s="6"/>
-      <c r="I57" s="6"/>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A58" s="6"/>
-      <c r="B58" s="6"/>
-      <c r="C58" s="6"/>
-      <c r="D58" s="6"/>
-      <c r="E58" s="6"/>
-      <c r="F58" s="6"/>
-      <c r="G58" s="6"/>
-      <c r="H58" s="6"/>
-      <c r="I58" s="6"/>
+      <c r="J56" s="14"/>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J57" s="14"/>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J58" s="14"/>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J59" s="14"/>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J60" s="14"/>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J61" s="14"/>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J62" s="14"/>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J63" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5588,8 +6099,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D600030-4003-4F44-BD14-20BD9D42365B}">
   <dimension ref="A1:M51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5798,11 +6309,11 @@
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="2" t="s">
+      <c r="E13" s="18"/>
+      <c r="F13" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="G13" s="6"/>
+      <c r="G13" s="20"/>
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
       <c r="J13" s="5"/>
@@ -5815,13 +6326,13 @@
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
-      <c r="E14" s="5" t="s">
+      <c r="E14" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="F14" s="11" t="s">
+      <c r="F14" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="G14" s="6"/>
+      <c r="G14" s="20"/>
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
       <c r="J14" s="5"/>
@@ -5834,13 +6345,13 @@
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
-      <c r="E15" s="5" t="s">
+      <c r="E15" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="F15" s="6" t="s">
+      <c r="F15" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="G15" s="6"/>
+      <c r="G15" s="20"/>
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
       <c r="J15" s="5"/>
@@ -5853,13 +6364,13 @@
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
-      <c r="E16" s="5" t="s">
+      <c r="E16" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="F16" s="6" t="s">
+      <c r="F16" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="G16" s="6"/>
+      <c r="G16" s="20"/>
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
       <c r="J16" s="5"/>
@@ -5883,13 +6394,13 @@
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
-      <c r="E18" s="5" t="s">
+      <c r="E18" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="F18" s="8" t="s">
+      <c r="F18" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="G18" s="6"/>
+      <c r="G18" s="20"/>
       <c r="H18" s="6"/>
       <c r="I18" s="6"/>
     </row>
@@ -5898,13 +6409,13 @@
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
-      <c r="E19" s="5" t="s">
+      <c r="E19" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="F19" s="11" t="s">
+      <c r="F19" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="G19" s="6"/>
+      <c r="G19" s="20"/>
       <c r="H19" s="6"/>
       <c r="I19" s="6"/>
     </row>
@@ -6272,7 +6783,7 @@
   <dimension ref="A1:BC65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="J5" sqref="J5:K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6313,8 +6824,8 @@
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="2" t="s">
+      <c r="J5" s="18"/>
+      <c r="K5" s="19" t="s">
         <v>44</v>
       </c>
       <c r="L5" s="5"/>
@@ -6380,10 +6891,10 @@
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
-      <c r="J6" s="5" t="s">
+      <c r="J6" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="K6" s="5" t="s">
+      <c r="K6" s="18" t="s">
         <v>47</v>
       </c>
       <c r="L6" s="5"/>
@@ -6451,10 +6962,10 @@
         <v>48</v>
       </c>
       <c r="I7" s="5"/>
-      <c r="J7" s="5" t="s">
+      <c r="J7" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="K7" s="5" t="s">
+      <c r="K7" s="18" t="s">
         <v>20</v>
       </c>
       <c r="L7" s="5"/>
@@ -9864,7 +10375,7 @@
   <dimension ref="A1:P57"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9927,7 +10438,7 @@
       <c r="E7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="17" t="s">
+      <c r="F7" s="25" t="s">
         <v>17</v>
       </c>
       <c r="G7" s="3"/>
@@ -11655,7 +12166,7 @@
       <c r="F17" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G17" s="18" t="s">
+      <c r="G17" s="17" t="s">
         <v>91</v>
       </c>
       <c r="H17" s="6"/>
@@ -11687,7 +12198,7 @@
       <c r="F19" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="G19" s="18" t="s">
+      <c r="G19" s="17" t="s">
         <v>20</v>
       </c>
       <c r="H19" s="6"/>
@@ -12172,8 +12683,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C82FD85-E493-4AC3-98EE-8D000540EFD3}">
   <dimension ref="A2:P58"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView topLeftCell="D8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12183,7 +12694,10 @@
     <col min="4" max="4" width="29.42578125" style="5" customWidth="1"/>
     <col min="5" max="5" width="42.85546875" style="5" customWidth="1"/>
     <col min="6" max="6" width="3" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="11.42578125" style="5"/>
+    <col min="7" max="10" width="11.42578125" style="5"/>
+    <col min="11" max="11" width="3.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" style="5" customWidth="1"/>
+    <col min="13" max="16384" width="11.42578125" style="5"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
@@ -12354,7 +12868,9 @@
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
+      <c r="L13" s="18" t="s">
+        <v>209</v>
+      </c>
       <c r="M13" s="3"/>
       <c r="N13" s="3"/>
       <c r="O13" s="3"/>
@@ -12379,7 +12895,9 @@
       <c r="I14" s="3"/>
       <c r="J14" s="10"/>
       <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
+      <c r="L14" s="18" t="s">
+        <v>212</v>
+      </c>
       <c r="M14" s="3"/>
       <c r="N14" s="3"/>
       <c r="O14" s="3"/>
@@ -12397,12 +12915,20 @@
       <c r="F15" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="G15" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="6"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="20"/>
+      <c r="J15" s="20"/>
+      <c r="K15" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="L15" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
@@ -12417,47 +12943,84 @@
       <c r="F16" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="G16" s="10" t="s">
+      <c r="G16" s="20" t="s">
         <v>102</v>
       </c>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H16" s="20"/>
+      <c r="I16" s="20"/>
+      <c r="J16" s="20"/>
+      <c r="K16" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="L16" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
       <c r="E17" s="7"/>
-      <c r="G17" s="18"/>
+      <c r="G17" s="21" t="s">
+        <v>213</v>
+      </c>
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
       <c r="J17" s="6"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K17" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="L17" s="19" t="s">
+        <v>210</v>
+      </c>
+      <c r="M17" s="3"/>
+      <c r="N17" s="3"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
-      <c r="G18" s="6"/>
+      <c r="G18" s="21" t="s">
+        <v>214</v>
+      </c>
       <c r="H18" s="6"/>
       <c r="I18" s="6"/>
       <c r="J18" s="6"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K18" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="L18" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="M18" s="3"/>
+      <c r="N18" s="3"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="7"/>
-      <c r="G19" s="18"/>
+      <c r="G19" s="21" t="s">
+        <v>215</v>
+      </c>
       <c r="H19" s="6"/>
       <c r="I19" s="6"/>
       <c r="J19" s="6"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K19" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="L19" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="N19" s="3"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
@@ -12468,8 +13031,16 @@
       <c r="H20" s="6"/>
       <c r="I20" s="6"/>
       <c r="J20" s="6"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K20" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="L20" s="19" t="s">
+        <v>211</v>
+      </c>
+      <c r="M20" s="3"/>
+      <c r="N20" s="3"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
@@ -12480,8 +13051,16 @@
       <c r="H21" s="6"/>
       <c r="I21" s="6"/>
       <c r="J21" s="6"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K21" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="L21" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="M21" s="3"/>
+      <c r="N21" s="3"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="6"/>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
@@ -12492,8 +13071,16 @@
       <c r="H22" s="6"/>
       <c r="I22" s="6"/>
       <c r="J22" s="6"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K22" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="L22" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
@@ -12504,8 +13091,16 @@
       <c r="H23" s="6"/>
       <c r="I23" s="6"/>
       <c r="J23" s="6"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K23" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="L23" s="22" t="s">
+        <v>216</v>
+      </c>
+      <c r="M23" s="6"/>
+      <c r="N23" s="6"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="6"/>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
@@ -12516,8 +13111,10 @@
       <c r="H24" s="6"/>
       <c r="I24" s="6"/>
       <c r="J24" s="6"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M24" s="6"/>
+      <c r="N24" s="6"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="6"/>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
@@ -12529,7 +13126,7 @@
       <c r="I25" s="6"/>
       <c r="J25" s="6"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="6"/>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
@@ -12541,7 +13138,7 @@
       <c r="I26" s="6"/>
       <c r="J26" s="6"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="6"/>
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
@@ -12553,7 +13150,7 @@
       <c r="I27" s="6"/>
       <c r="J27" s="6"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="6"/>
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
@@ -12565,7 +13162,7 @@
       <c r="I28" s="6"/>
       <c r="J28" s="6"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
@@ -12577,7 +13174,7 @@
       <c r="I29" s="6"/>
       <c r="J29" s="6"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="6"/>
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
@@ -12589,7 +13186,7 @@
       <c r="I30" s="6"/>
       <c r="J30" s="6"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="6"/>
       <c r="B31" s="6"/>
       <c r="C31" s="6"/>
@@ -12601,7 +13198,7 @@
       <c r="I31" s="6"/>
       <c r="J31" s="6"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="6"/>
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
@@ -12935,7 +13532,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3897752D-E3F5-4B9F-AC20-3D10E360EA9E}">
   <dimension ref="A2:O58"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
@@ -13178,7 +13775,7 @@
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
-      <c r="F17" s="18"/>
+      <c r="F17" s="17"/>
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
@@ -13198,7 +13795,7 @@
       <c r="B19" s="3"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
-      <c r="F19" s="18"/>
+      <c r="F19" s="17"/>
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
       <c r="I19" s="6"/>
@@ -13854,7 +14451,7 @@
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
-      <c r="F17" s="18"/>
+      <c r="F17" s="17"/>
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
@@ -13874,7 +14471,7 @@
       <c r="B19" s="3"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
-      <c r="F19" s="18"/>
+      <c r="F19" s="17"/>
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
       <c r="I19" s="6"/>

</xml_diff>